<commit_message>
Change power screw terminals
</commit_message>
<xml_diff>
--- a/Source/Project Outputs for RUMBA_plus/RUMBA_plus_BOM_1_3_1.xlsx
+++ b/Source/Project Outputs for RUMBA_plus/RUMBA_plus_BOM_1_3_1.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\RUMBA-Plus\Source\Project Outputs for RUMBA_plus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Git\RUMBA-Plus\Source\Project Outputs for RUMBA_plus\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAD8432-DB7B-4F5C-8E06-13E6C34AA2D0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22275" windowHeight="16230" xr2:uid="{FD7B852F-20E6-4A44-AE1F-F610DC299137}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="261">
   <si>
     <t>Designator</t>
   </si>
@@ -362,12 +363,6 @@
     <t>Screw Terminal 5mm 2-Way</t>
   </si>
   <si>
-    <t>1935776</t>
-  </si>
-  <si>
-    <t>277-6405-ND</t>
-  </si>
-  <si>
     <t>Header, 5-Pin</t>
   </si>
   <si>
@@ -801,6 +796,18 @@
   </si>
   <si>
     <t>SSB44-E3/52TGICT-ND</t>
+  </si>
+  <si>
+    <t>Rising Cage Clamp</t>
+  </si>
+  <si>
+    <t>TE Connectivity AMP Connectors</t>
+  </si>
+  <si>
+    <t>282856-2</t>
+  </si>
+  <si>
+    <t>A98355-ND</t>
   </si>
 </sst>
 </file>
@@ -1745,7 +1752,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G23" sqref="G23:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,7 +1821,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="1"/>
@@ -1857,7 +1864,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -1889,7 +1896,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>45</v>
@@ -1921,7 +1928,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>24</v>
@@ -1953,7 +1960,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -1985,7 +1992,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>36</v>
@@ -2081,7 +2088,7 @@
         <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>65</v>
@@ -2113,7 +2120,7 @@
         <v>69</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>70</v>
@@ -2145,13 +2152,13 @@
         <v>73</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -2160,27 +2167,27 @@
         <v>14</v>
       </c>
       <c r="G13" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -2192,7 +2199,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="1"/>
@@ -2232,7 +2239,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>80</v>
@@ -2250,7 +2257,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="1"/>
@@ -2308,7 +2315,7 @@
         <v>14</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="1"/>
@@ -2334,7 +2341,7 @@
         <v>14</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="1"/>
@@ -2441,7 +2448,7 @@
         <v>111</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>111</v>
+        <v>257</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>
@@ -2449,31 +2456,29 @@
       <c r="E23" s="2">
         <v>3</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="3" t="s">
-        <v>77</v>
+        <v>258</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>112</v>
+        <v>259</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>113</v>
+      <c r="J23" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>13</v>
@@ -2485,7 +2490,7 @@
         <v>14</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="1"/>
@@ -2493,10 +2498,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="1" t="s">
@@ -2509,30 +2514,30 @@
         <v>14</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>126</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
@@ -2544,27 +2549,27 @@
         <v>47</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
@@ -2573,30 +2578,30 @@
         <v>14</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
@@ -2605,27 +2610,27 @@
         <v>14</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>13</v>
@@ -2637,27 +2642,27 @@
         <v>14</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>13</v>
@@ -2669,27 +2674,27 @@
         <v>14</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2">
@@ -2697,27 +2702,27 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>13</v>
@@ -2729,30 +2734,30 @@
         <v>13</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
@@ -2764,27 +2769,27 @@
         <v>32</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="E34" s="2">
         <v>13</v>
@@ -2796,27 +2801,27 @@
         <v>32</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="E35" s="2">
         <v>1</v>
@@ -2828,27 +2833,27 @@
         <v>32</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="E36" s="2">
         <v>12</v>
@@ -2860,27 +2865,27 @@
         <v>32</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="E37" s="2">
         <v>15</v>
@@ -2892,27 +2897,27 @@
         <v>32</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E38" s="2">
         <v>6</v>
@@ -2924,27 +2929,27 @@
         <v>32</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="E39" s="2">
         <v>1</v>
@@ -2956,27 +2961,27 @@
         <v>32</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="E40" s="2">
         <v>1</v>
@@ -2988,27 +2993,27 @@
         <v>32</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E41" s="2">
         <v>8</v>
@@ -3020,24 +3025,24 @@
         <v>32</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>13</v>
@@ -3049,27 +3054,27 @@
         <v>14</v>
       </c>
       <c r="G42" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>13</v>
@@ -3081,27 +3086,27 @@
         <v>13</v>
       </c>
       <c r="G43" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -3113,27 +3118,27 @@
         <v>13</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>13</v>
@@ -3145,27 +3150,27 @@
         <v>13</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>13</v>
@@ -3177,27 +3182,27 @@
         <v>13</v>
       </c>
       <c r="G46" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>13</v>
@@ -3209,27 +3214,27 @@
         <v>14</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H47" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>13</v>
@@ -3241,7 +3246,7 @@
         <v>14</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="1"/>
@@ -3249,13 +3254,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>13</v>
@@ -3267,7 +3272,7 @@
         <v>14</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="1"/>
@@ -3275,13 +3280,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>226</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>13</v>
@@ -3293,16 +3298,16 @@
         <v>14</v>
       </c>
       <c r="G50" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="14" t="s">
         <v>227</v>
-      </c>
-      <c r="H50" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J50" s="14" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3359,86 +3364,83 @@
     <hyperlink ref="G22" r:id="rId50" tooltip="Component" display="'Phoenix Contact" xr:uid="{8E33D070-85B3-45B0-9D72-9DEA8C64A27A}"/>
     <hyperlink ref="H22" r:id="rId51" tooltip="Manufacturer" display="'1751248" xr:uid="{27069FCF-26AC-4F60-8EDA-B73F085A841F}"/>
     <hyperlink ref="J22" r:id="rId52" tooltip="Supplier" display="'277-5719-ND" xr:uid="{072D2A82-ED4A-4927-B341-58FB066FBA76}"/>
-    <hyperlink ref="G23" r:id="rId53" tooltip="Component" display="'Phoenix Contact" xr:uid="{3EEC6F74-AAB0-4E68-B2F2-BE3D1EBF9214}"/>
-    <hyperlink ref="H23" r:id="rId54" tooltip="Manufacturer" display="'1935776" xr:uid="{D0E24E1C-FC1B-4C94-BB84-CDBDFD0B2271}"/>
-    <hyperlink ref="J23" r:id="rId55" tooltip="Supplier" display="'277-6405-ND" xr:uid="{57E198F2-03D9-4C1E-98E3-D8E88342CE06}"/>
-    <hyperlink ref="G48" r:id="rId56" tooltip="Component" display="'Loading..." xr:uid="{99534DDB-1774-407E-BD72-7D3668C9B630}"/>
-    <hyperlink ref="G24" r:id="rId57" tooltip="Component" display="'Loading..." xr:uid="{D760A977-B9E1-4C61-8FAE-CB62F2BEFBBD}"/>
-    <hyperlink ref="G25" r:id="rId58" tooltip="Component" display="'Molex, LLC" xr:uid="{0F5FD788-F564-4A60-A2B5-109732D6ED30}"/>
-    <hyperlink ref="H25" r:id="rId59" tooltip="Manufacturer" display="'1050170001" xr:uid="{B10606C0-E169-41AC-9B1B-F046E7E8510B}"/>
-    <hyperlink ref="J25" r:id="rId60" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{0989CB1B-579D-4020-A5FD-0E4ABE9D7703}"/>
-    <hyperlink ref="G26" r:id="rId61" tooltip="Component" display="'Murata Electronics North America" xr:uid="{D4304DAD-AEA9-4A0B-9023-C8C19E9FD2F3}"/>
-    <hyperlink ref="H26" r:id="rId62" tooltip="Manufacturer" display="'BLM21PG221SN1D" xr:uid="{63933F83-B76B-44CD-8CE8-1865C9C817D7}"/>
-    <hyperlink ref="J26" r:id="rId63" tooltip="Supplier" display="'490-1054-1-ND" xr:uid="{1E4D4793-B327-43AA-8F6C-D834CE45C90D}"/>
-    <hyperlink ref="G27" r:id="rId64" tooltip="Component" display="'Bourns Inc." xr:uid="{5E42FB16-A764-47DE-9A5B-D5B7FB62B66C}"/>
-    <hyperlink ref="H27" r:id="rId65" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{2CD86F8E-580A-44C3-A25C-C9769E024EF7}"/>
-    <hyperlink ref="J27" r:id="rId66" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{13951AE0-C7C0-43BA-BE32-C42CFD079DC4}"/>
-    <hyperlink ref="G28" r:id="rId67" tooltip="Component" display="'Bourns Inc." xr:uid="{3A3BA2F0-D76C-4591-8243-99CD334215D0}"/>
-    <hyperlink ref="H28" r:id="rId68" tooltip="Manufacturer" display="'SRN8040TA-470M" xr:uid="{9393FD5F-F406-4DDA-B2F6-A5087E59B162}"/>
-    <hyperlink ref="J28" r:id="rId69" tooltip="Supplier" display="'SRN8040TA-470MCT-ND" xr:uid="{BE956B5E-DBA7-4876-99D7-BD2953EE7A3E}"/>
-    <hyperlink ref="G29" r:id="rId70" tooltip="Component" display="'Lite-On Inc." xr:uid="{1BFC70D3-D369-4F4A-BC39-F51EC41C90E5}"/>
-    <hyperlink ref="H29" r:id="rId71" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{961D9B5D-F3D3-46C6-9E7D-993401706C55}"/>
-    <hyperlink ref="J29" r:id="rId72" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{4989D82B-EDE2-45AD-8316-0BE497E40D5B}"/>
-    <hyperlink ref="G30" r:id="rId73" tooltip="Component" display="'Lite-On Inc." xr:uid="{639D4ACD-5799-402D-803C-17A777CAFADE}"/>
-    <hyperlink ref="H30" r:id="rId74" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{2413BFA6-6008-41BC-AB9E-D0CADB0841F0}"/>
-    <hyperlink ref="J30" r:id="rId75" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{94979B37-F572-4850-BEF9-C3428194D2AD}"/>
-    <hyperlink ref="G33" r:id="rId76" tooltip="Component" display="'Yageo" xr:uid="{08B992B2-5FFD-468F-8C37-F5E0E55827CA}"/>
-    <hyperlink ref="H33" r:id="rId77" tooltip="Manufacturer" display="'RC0603FR-071ML" xr:uid="{7D006478-1E4D-4D42-85C7-033ABCB72197}"/>
-    <hyperlink ref="J33" r:id="rId78" tooltip="Supplier" display="'311-1.00MHRDKR-ND" xr:uid="{85B8248E-2152-4AEE-9145-234BD60567AA}"/>
-    <hyperlink ref="G36" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{7A3BC117-10FA-4978-95C8-B8FEC528AE8C}"/>
-    <hyperlink ref="H36" r:id="rId80" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{3E10DF3F-5206-4953-A38F-24F8BF7A0D63}"/>
-    <hyperlink ref="J36" r:id="rId81" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{6A20EF17-382F-49C2-A769-EBF46975E659}"/>
-    <hyperlink ref="G37" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{5F9D81C6-4FA4-41B4-83FC-838B41BF9D63}"/>
-    <hyperlink ref="H37" r:id="rId83" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{EC5C9DBC-CA01-4E84-8AB1-A1E011F4969C}"/>
-    <hyperlink ref="J37" r:id="rId84" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{9EE26DE7-963D-4581-A9CD-06D42E170F76}"/>
-    <hyperlink ref="G39" r:id="rId85" tooltip="Component" display="'Yageo" xr:uid="{7CC16B12-D4DA-42BE-B00E-AF45B84234CE}"/>
-    <hyperlink ref="H39" r:id="rId86" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{4B29041A-5D4F-4E9F-85F0-FE3EC9EECF7F}"/>
-    <hyperlink ref="J39" r:id="rId87" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{91882D23-815E-4187-9AAD-24127BF44ECE}"/>
-    <hyperlink ref="G41" r:id="rId88" tooltip="Component" display="'Yageo" xr:uid="{14BC76A9-9358-431A-80A8-D0CD2925110D}"/>
-    <hyperlink ref="H41" r:id="rId89" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{0C32B3D1-D5BC-425A-9128-C60912E9D570}"/>
-    <hyperlink ref="J41" r:id="rId90" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{F851E52C-EEB8-4A75-9E50-490FA833C07A}"/>
-    <hyperlink ref="G34" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{04DAF956-9707-421B-9902-660D148AD02A}"/>
-    <hyperlink ref="H34" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{8885096B-1925-40B5-9B6A-8A913F04A0E5}"/>
-    <hyperlink ref="J34" r:id="rId93" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{008657BB-878C-496B-AC2C-CAF672731554}"/>
-    <hyperlink ref="G35" r:id="rId94" tooltip="Component" display="'Yageo" xr:uid="{2FBCF6ED-10E7-4215-9E32-249EF6E45BAE}"/>
-    <hyperlink ref="H35" r:id="rId95" tooltip="Manufacturer" display="'RC0603FR-0753K6L" xr:uid="{D20F714A-064B-47F9-A242-40BB25004199}"/>
-    <hyperlink ref="J35" r:id="rId96" tooltip="Supplier" display="'311-53.6KHRCT-ND" xr:uid="{B0FC8B5D-3CA9-41D6-978F-C4C739948B27}"/>
-    <hyperlink ref="G38" r:id="rId97" tooltip="Component" display="'Yageo" xr:uid="{D05D8D23-0FD7-4EB0-82B5-012867FB4A29}"/>
-    <hyperlink ref="H38" r:id="rId98" tooltip="Manufacturer" display="'RC0603JR-074K7L" xr:uid="{487CC820-6958-4015-8E07-2B1B6917AB28}"/>
-    <hyperlink ref="J38" r:id="rId99" tooltip="Supplier" display="'311-4.7KGRCT-ND" xr:uid="{EB3C4C30-1438-46A2-85B2-C2570D6C8061}"/>
-    <hyperlink ref="G40" r:id="rId100" tooltip="Component" display="'Yageo" xr:uid="{83B23BCD-9D2D-4244-A8D9-855CBC334E2E}"/>
-    <hyperlink ref="H40" r:id="rId101" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{CC682DC2-92DA-4617-89AC-DBE9484E8EB3}"/>
-    <hyperlink ref="J40" r:id="rId102" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{77F80A98-4E5F-42FB-8366-09D154AF8FBF}"/>
-    <hyperlink ref="G42" r:id="rId103" tooltip="Component" display="'APEM Inc." xr:uid="{8DA80FE1-AD41-41A1-AF5B-29C7AE5C205A}"/>
-    <hyperlink ref="H42" r:id="rId104" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{3E38DB83-F083-4406-9B4E-413981B63A75}"/>
-    <hyperlink ref="J42" r:id="rId105" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{801CE691-B5ED-4969-8922-A4400E0A0F04}"/>
-    <hyperlink ref="G46" r:id="rId106" tooltip="Component" display="'Alpha &amp; Omega Semiconductor Inc." xr:uid="{B20D082B-86E0-455B-948A-E56AA2128005}"/>
-    <hyperlink ref="H46" r:id="rId107" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{FBD90C73-9CDC-45FA-A900-851BCE6704DB}"/>
-    <hyperlink ref="J46" r:id="rId108" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{E2C42AC0-6C55-40A7-8049-274675441D9B}"/>
-    <hyperlink ref="G47" r:id="rId109" tooltip="Component" display="'STMicroelectronics" xr:uid="{785209C2-D378-474E-97B4-42C17DE72E9A}"/>
-    <hyperlink ref="H47" r:id="rId110" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{98791FDC-D4C5-4551-847A-1B45F6539CBF}"/>
-    <hyperlink ref="J47" r:id="rId111" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{E2F9A172-96B8-4383-B884-A6A1414CF4A7}"/>
-    <hyperlink ref="G43" r:id="rId112" tooltip="Component" display="'Microchip Technology" xr:uid="{D0D2B9E1-7600-421F-BB55-D5E4CF817D2B}"/>
-    <hyperlink ref="H43" r:id="rId113" tooltip="Manufacturer" display="'ATMEGA2560-16AU" xr:uid="{3090BB5A-0847-4847-AA65-518ED9057C4F}"/>
-    <hyperlink ref="J43" r:id="rId114" tooltip="Supplier" display="'ATMEGA2560-16AU-ND" xr:uid="{21D45919-A9D2-4071-80EE-68A0A0D8492D}"/>
-    <hyperlink ref="G44" r:id="rId115" tooltip="Component" display="'Microchip Technology" xr:uid="{21BB9AC5-9AC5-4C89-A6B2-5C2DD94EEA56}"/>
-    <hyperlink ref="H44" r:id="rId116" tooltip="Manufacturer" display="'ATMEGA16U2-AU" xr:uid="{71DEC28B-A006-4DF5-BB66-FBB703DC7EFC}"/>
-    <hyperlink ref="J44" r:id="rId117" tooltip="Supplier" display="'ATMEGA16U2-AU-ND" xr:uid="{752CFA2A-364D-4706-BD90-0EF7750AEE11}"/>
-    <hyperlink ref="G45" r:id="rId118" tooltip="Component" display="'Alpha &amp; Omega Semiconductor Inc." xr:uid="{BE4F2880-1B87-45DB-B4B9-3BC68B11948D}"/>
-    <hyperlink ref="H45" r:id="rId119" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{00CF3BA0-9B64-4C44-A4CC-99B3C12958E9}"/>
-    <hyperlink ref="J45" r:id="rId120" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{CE07DCE4-81F1-4E37-AE55-1FF5C4A25DD5}"/>
-    <hyperlink ref="G49" r:id="rId121" tooltip="Component" display="'Loading..." xr:uid="{7FFD9829-C7FD-48AB-9008-67414D5F3A9B}"/>
-    <hyperlink ref="G50" r:id="rId122" tooltip="Component" display="'EPSON" xr:uid="{307A7C81-BA6D-4A04-84C8-3CD77AE1DB8E}"/>
-    <hyperlink ref="H50" r:id="rId123" tooltip="Manufacturer" display="'FA-238 16.0000MB-C3" xr:uid="{38323FE7-4E4F-4998-8A1E-5F7113325831}"/>
-    <hyperlink ref="J50" r:id="rId124" tooltip="Supplier" display="'SER3686CT-ND" xr:uid="{225B874A-BB17-40EC-AD86-2ADBDA9439C8}"/>
-    <hyperlink ref="G32" r:id="rId125" tooltip="Component" xr:uid="{8C0B0BB1-B33C-4761-A4B1-3E86C1AAAB94}"/>
-    <hyperlink ref="H32" r:id="rId126" tooltip="Manufacturer" xr:uid="{6F8EF1F8-2416-4CF4-AA0A-77819531DF15}"/>
-    <hyperlink ref="J13" r:id="rId127" tooltip="Supplier" display="'1655-1602-1-ND" xr:uid="{13BBE097-86BB-46AD-BF92-9097170A4C18}"/>
+    <hyperlink ref="G48" r:id="rId53" tooltip="Component" display="'Loading..." xr:uid="{99534DDB-1774-407E-BD72-7D3668C9B630}"/>
+    <hyperlink ref="G24" r:id="rId54" tooltip="Component" display="'Loading..." xr:uid="{D760A977-B9E1-4C61-8FAE-CB62F2BEFBBD}"/>
+    <hyperlink ref="G25" r:id="rId55" tooltip="Component" display="'Molex, LLC" xr:uid="{0F5FD788-F564-4A60-A2B5-109732D6ED30}"/>
+    <hyperlink ref="H25" r:id="rId56" tooltip="Manufacturer" display="'1050170001" xr:uid="{B10606C0-E169-41AC-9B1B-F046E7E8510B}"/>
+    <hyperlink ref="J25" r:id="rId57" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{0989CB1B-579D-4020-A5FD-0E4ABE9D7703}"/>
+    <hyperlink ref="G26" r:id="rId58" tooltip="Component" display="'Murata Electronics North America" xr:uid="{D4304DAD-AEA9-4A0B-9023-C8C19E9FD2F3}"/>
+    <hyperlink ref="H26" r:id="rId59" tooltip="Manufacturer" display="'BLM21PG221SN1D" xr:uid="{63933F83-B76B-44CD-8CE8-1865C9C817D7}"/>
+    <hyperlink ref="J26" r:id="rId60" tooltip="Supplier" display="'490-1054-1-ND" xr:uid="{1E4D4793-B327-43AA-8F6C-D834CE45C90D}"/>
+    <hyperlink ref="G27" r:id="rId61" tooltip="Component" display="'Bourns Inc." xr:uid="{5E42FB16-A764-47DE-9A5B-D5B7FB62B66C}"/>
+    <hyperlink ref="H27" r:id="rId62" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{2CD86F8E-580A-44C3-A25C-C9769E024EF7}"/>
+    <hyperlink ref="J27" r:id="rId63" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{13951AE0-C7C0-43BA-BE32-C42CFD079DC4}"/>
+    <hyperlink ref="G28" r:id="rId64" tooltip="Component" display="'Bourns Inc." xr:uid="{3A3BA2F0-D76C-4591-8243-99CD334215D0}"/>
+    <hyperlink ref="H28" r:id="rId65" tooltip="Manufacturer" display="'SRN8040TA-470M" xr:uid="{9393FD5F-F406-4DDA-B2F6-A5087E59B162}"/>
+    <hyperlink ref="J28" r:id="rId66" tooltip="Supplier" display="'SRN8040TA-470MCT-ND" xr:uid="{BE956B5E-DBA7-4876-99D7-BD2953EE7A3E}"/>
+    <hyperlink ref="G29" r:id="rId67" tooltip="Component" display="'Lite-On Inc." xr:uid="{1BFC70D3-D369-4F4A-BC39-F51EC41C90E5}"/>
+    <hyperlink ref="H29" r:id="rId68" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{961D9B5D-F3D3-46C6-9E7D-993401706C55}"/>
+    <hyperlink ref="J29" r:id="rId69" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{4989D82B-EDE2-45AD-8316-0BE497E40D5B}"/>
+    <hyperlink ref="G30" r:id="rId70" tooltip="Component" display="'Lite-On Inc." xr:uid="{639D4ACD-5799-402D-803C-17A777CAFADE}"/>
+    <hyperlink ref="H30" r:id="rId71" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{2413BFA6-6008-41BC-AB9E-D0CADB0841F0}"/>
+    <hyperlink ref="J30" r:id="rId72" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{94979B37-F572-4850-BEF9-C3428194D2AD}"/>
+    <hyperlink ref="G33" r:id="rId73" tooltip="Component" display="'Yageo" xr:uid="{08B992B2-5FFD-468F-8C37-F5E0E55827CA}"/>
+    <hyperlink ref="H33" r:id="rId74" tooltip="Manufacturer" display="'RC0603FR-071ML" xr:uid="{7D006478-1E4D-4D42-85C7-033ABCB72197}"/>
+    <hyperlink ref="J33" r:id="rId75" tooltip="Supplier" display="'311-1.00MHRDKR-ND" xr:uid="{85B8248E-2152-4AEE-9145-234BD60567AA}"/>
+    <hyperlink ref="G36" r:id="rId76" tooltip="Component" display="'Yageo" xr:uid="{7A3BC117-10FA-4978-95C8-B8FEC528AE8C}"/>
+    <hyperlink ref="H36" r:id="rId77" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{3E10DF3F-5206-4953-A38F-24F8BF7A0D63}"/>
+    <hyperlink ref="J36" r:id="rId78" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{6A20EF17-382F-49C2-A769-EBF46975E659}"/>
+    <hyperlink ref="G37" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{5F9D81C6-4FA4-41B4-83FC-838B41BF9D63}"/>
+    <hyperlink ref="H37" r:id="rId80" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{EC5C9DBC-CA01-4E84-8AB1-A1E011F4969C}"/>
+    <hyperlink ref="J37" r:id="rId81" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{9EE26DE7-963D-4581-A9CD-06D42E170F76}"/>
+    <hyperlink ref="G39" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{7CC16B12-D4DA-42BE-B00E-AF45B84234CE}"/>
+    <hyperlink ref="H39" r:id="rId83" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{4B29041A-5D4F-4E9F-85F0-FE3EC9EECF7F}"/>
+    <hyperlink ref="J39" r:id="rId84" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{91882D23-815E-4187-9AAD-24127BF44ECE}"/>
+    <hyperlink ref="G41" r:id="rId85" tooltip="Component" display="'Yageo" xr:uid="{14BC76A9-9358-431A-80A8-D0CD2925110D}"/>
+    <hyperlink ref="H41" r:id="rId86" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{0C32B3D1-D5BC-425A-9128-C60912E9D570}"/>
+    <hyperlink ref="J41" r:id="rId87" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{F851E52C-EEB8-4A75-9E50-490FA833C07A}"/>
+    <hyperlink ref="G34" r:id="rId88" tooltip="Component" display="'Yageo" xr:uid="{04DAF956-9707-421B-9902-660D148AD02A}"/>
+    <hyperlink ref="H34" r:id="rId89" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{8885096B-1925-40B5-9B6A-8A913F04A0E5}"/>
+    <hyperlink ref="J34" r:id="rId90" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{008657BB-878C-496B-AC2C-CAF672731554}"/>
+    <hyperlink ref="G35" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{2FBCF6ED-10E7-4215-9E32-249EF6E45BAE}"/>
+    <hyperlink ref="H35" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-0753K6L" xr:uid="{D20F714A-064B-47F9-A242-40BB25004199}"/>
+    <hyperlink ref="J35" r:id="rId93" tooltip="Supplier" display="'311-53.6KHRCT-ND" xr:uid="{B0FC8B5D-3CA9-41D6-978F-C4C739948B27}"/>
+    <hyperlink ref="G38" r:id="rId94" tooltip="Component" display="'Yageo" xr:uid="{D05D8D23-0FD7-4EB0-82B5-012867FB4A29}"/>
+    <hyperlink ref="H38" r:id="rId95" tooltip="Manufacturer" display="'RC0603JR-074K7L" xr:uid="{487CC820-6958-4015-8E07-2B1B6917AB28}"/>
+    <hyperlink ref="J38" r:id="rId96" tooltip="Supplier" display="'311-4.7KGRCT-ND" xr:uid="{EB3C4C30-1438-46A2-85B2-C2570D6C8061}"/>
+    <hyperlink ref="G40" r:id="rId97" tooltip="Component" display="'Yageo" xr:uid="{83B23BCD-9D2D-4244-A8D9-855CBC334E2E}"/>
+    <hyperlink ref="H40" r:id="rId98" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{CC682DC2-92DA-4617-89AC-DBE9484E8EB3}"/>
+    <hyperlink ref="J40" r:id="rId99" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{77F80A98-4E5F-42FB-8366-09D154AF8FBF}"/>
+    <hyperlink ref="G42" r:id="rId100" tooltip="Component" display="'APEM Inc." xr:uid="{8DA80FE1-AD41-41A1-AF5B-29C7AE5C205A}"/>
+    <hyperlink ref="H42" r:id="rId101" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{3E38DB83-F083-4406-9B4E-413981B63A75}"/>
+    <hyperlink ref="J42" r:id="rId102" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{801CE691-B5ED-4969-8922-A4400E0A0F04}"/>
+    <hyperlink ref="G46" r:id="rId103" tooltip="Component" display="'Alpha &amp; Omega Semiconductor Inc." xr:uid="{B20D082B-86E0-455B-948A-E56AA2128005}"/>
+    <hyperlink ref="H46" r:id="rId104" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{FBD90C73-9CDC-45FA-A900-851BCE6704DB}"/>
+    <hyperlink ref="J46" r:id="rId105" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{E2C42AC0-6C55-40A7-8049-274675441D9B}"/>
+    <hyperlink ref="G47" r:id="rId106" tooltip="Component" display="'STMicroelectronics" xr:uid="{785209C2-D378-474E-97B4-42C17DE72E9A}"/>
+    <hyperlink ref="H47" r:id="rId107" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{98791FDC-D4C5-4551-847A-1B45F6539CBF}"/>
+    <hyperlink ref="J47" r:id="rId108" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{E2F9A172-96B8-4383-B884-A6A1414CF4A7}"/>
+    <hyperlink ref="G43" r:id="rId109" tooltip="Component" display="'Microchip Technology" xr:uid="{D0D2B9E1-7600-421F-BB55-D5E4CF817D2B}"/>
+    <hyperlink ref="H43" r:id="rId110" tooltip="Manufacturer" display="'ATMEGA2560-16AU" xr:uid="{3090BB5A-0847-4847-AA65-518ED9057C4F}"/>
+    <hyperlink ref="J43" r:id="rId111" tooltip="Supplier" display="'ATMEGA2560-16AU-ND" xr:uid="{21D45919-A9D2-4071-80EE-68A0A0D8492D}"/>
+    <hyperlink ref="G44" r:id="rId112" tooltip="Component" display="'Microchip Technology" xr:uid="{21BB9AC5-9AC5-4C89-A6B2-5C2DD94EEA56}"/>
+    <hyperlink ref="H44" r:id="rId113" tooltip="Manufacturer" display="'ATMEGA16U2-AU" xr:uid="{71DEC28B-A006-4DF5-BB66-FBB703DC7EFC}"/>
+    <hyperlink ref="J44" r:id="rId114" tooltip="Supplier" display="'ATMEGA16U2-AU-ND" xr:uid="{752CFA2A-364D-4706-BD90-0EF7750AEE11}"/>
+    <hyperlink ref="G45" r:id="rId115" tooltip="Component" display="'Alpha &amp; Omega Semiconductor Inc." xr:uid="{BE4F2880-1B87-45DB-B4B9-3BC68B11948D}"/>
+    <hyperlink ref="H45" r:id="rId116" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{00CF3BA0-9B64-4C44-A4CC-99B3C12958E9}"/>
+    <hyperlink ref="J45" r:id="rId117" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{CE07DCE4-81F1-4E37-AE55-1FF5C4A25DD5}"/>
+    <hyperlink ref="G49" r:id="rId118" tooltip="Component" display="'Loading..." xr:uid="{7FFD9829-C7FD-48AB-9008-67414D5F3A9B}"/>
+    <hyperlink ref="G50" r:id="rId119" tooltip="Component" display="'EPSON" xr:uid="{307A7C81-BA6D-4A04-84C8-3CD77AE1DB8E}"/>
+    <hyperlink ref="H50" r:id="rId120" tooltip="Manufacturer" display="'FA-238 16.0000MB-C3" xr:uid="{38323FE7-4E4F-4998-8A1E-5F7113325831}"/>
+    <hyperlink ref="J50" r:id="rId121" tooltip="Supplier" display="'SER3686CT-ND" xr:uid="{225B874A-BB17-40EC-AD86-2ADBDA9439C8}"/>
+    <hyperlink ref="G32" r:id="rId122" tooltip="Component" xr:uid="{8C0B0BB1-B33C-4761-A4B1-3E86C1AAAB94}"/>
+    <hyperlink ref="H32" r:id="rId123" tooltip="Manufacturer" xr:uid="{6F8EF1F8-2416-4CF4-AA0A-77819531DF15}"/>
+    <hyperlink ref="J13" r:id="rId124" tooltip="Supplier" display="'1655-1602-1-ND" xr:uid="{13BBE097-86BB-46AD-BF92-9097170A4C18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="219" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId128"/>
+  <pageSetup paperSize="219" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId125"/>
   <tableParts count="1">
-    <tablePart r:id="rId129"/>
+    <tablePart r:id="rId126"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>